<commit_message>
trying to bypass .lock which doesn't enable to push freexe/ and /site/
</commit_message>
<xml_diff>
--- a/posts/whoami/data.xlsx
+++ b/posts/whoami/data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KSE\Projects\Shizukana Machi\_posts\2023-07-24-whoami\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KSE\Projects\kotori\posts\whoami\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AA10F0-8103-4E31-85FA-68658B6346BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4E4D6E-56DC-4EF7-A8AD-AA5D3845C59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -453,12 +453,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F55" sqref="F54:F55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +749,7 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1">
@@ -1191,7 +1189,7 @@
       <c r="A24" s="1">
         <v>2018</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C24" s="1" t="s">

</xml_diff>